<commit_message>
made a lot of changes
</commit_message>
<xml_diff>
--- a/generator/data/generated_business_labels_map_maps.xlsx
+++ b/generator/data/generated_business_labels_map_maps.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">i_econ_stop_business</t>
   </si>
   <si>
-    <t xml:space="preserve">No, operations were always running</t>
+    <t xml:space="preserve">Never shutdown</t>
   </si>
   <si>
     <t xml:space="preserve">होइन, अपरेशनहरू सँधै चलिरहेका थिए</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">i_econ_stop_business__1</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, temporarily stopped operations</t>
+    <t xml:space="preserve">Temporarily shutdown during the pandemic</t>
   </si>
   <si>
     <t xml:space="preserve">हो, अस्थायी रूपमा सञ्चालनहरू बन्द गरियो</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">i_econ_stop_business__2</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, permanently stopped</t>
+    <t xml:space="preserve">Permanently shutdown during the pandemic</t>
   </si>
   <si>
     <t xml:space="preserve">हो, स्थायी रूपमा रोकियो</t>
@@ -637,7 +637,7 @@
     <t xml:space="preserve">o_do_u_know_of_gov_schemes</t>
   </si>
   <si>
-    <t xml:space="preserve">I am not aware of such government schemes.</t>
+    <t xml:space="preserve">Not aware of any government schemes</t>
   </si>
   <si>
     <t xml:space="preserve">म त्यस्ता सरकारी योजनाहरूको बारेमा सचेत छैन।</t>
@@ -649,7 +649,7 @@
     <t xml:space="preserve">o_do_u_know_of_gov_schemes__1</t>
   </si>
   <si>
-    <t xml:space="preserve">I am aware about such schemes but haven’t used any.</t>
+    <t xml:space="preserve">Aware about government schemes but haven’t used any</t>
   </si>
   <si>
     <t xml:space="preserve"> मैले कुनै सरकारी योजना प्रयोग गरेको छैन तर मलाई त्यस्ता योजनाहरूको बारेमा थाहा छ।</t>
@@ -658,7 +658,7 @@
     <t xml:space="preserve">o_do_u_know_of_gov_schemes__2</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes, I have used one or more government schemes.</t>
+    <t xml:space="preserve">Have used one or more government schemes</t>
   </si>
   <si>
     <t xml:space="preserve">मैले एक वा बढी सरकारी योजनाहरू प्रयोग गरेको छु।</t>
@@ -1516,25 +1516,7 @@
     <t xml:space="preserve">o_rcvry_biggest_diffclties__2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ensuring health and safety measures for employees and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">guests</t>
-    </r>
+    <t xml:space="preserve">Ensuring health and safety measures for employees and guests</t>
   </si>
   <si>
     <t xml:space="preserve">पाहुनाहरू र पर्यटकहरूको लागि स्वास्थ्य र सुरक्षा उपायहरू सुनिश्चित गर्ने </t>
@@ -1615,7 +1597,7 @@
     <t xml:space="preserve">o_expectd_problms_next_6_mnths__2</t>
   </si>
   <si>
-    <t xml:space="preserve">Will have difficulties in paying its taxes</t>
+    <t xml:space="preserve">Will have difficulties in paying taxes</t>
   </si>
   <si>
     <t xml:space="preserve">मेरो व्यवसायलाई यसको करहरू तिर्नमा कठिनाइ हुनेछ</t>
@@ -1624,7 +1606,7 @@
     <t xml:space="preserve">o_expectd_problms_next_6_mnths__3</t>
   </si>
   <si>
-    <t xml:space="preserve">Will have difficulties in covering its operating costs</t>
+    <t xml:space="preserve">Will have difficulties in covering operating costs</t>
   </si>
   <si>
     <t xml:space="preserve">मेरो व्यवसायलाई यसको अपरेटिंग लागतहरू कभर गर्न कठिनाइ हुनेछ</t>
@@ -1642,7 +1624,7 @@
     <t xml:space="preserve">o_expectd_problms_next_6_mnths__5</t>
   </si>
   <si>
-    <t xml:space="preserve">Will have difficulties in getting enough customers required for its survival</t>
+    <t xml:space="preserve">Will have difficulties in getting enough customers required for survival</t>
   </si>
   <si>
     <t xml:space="preserve">मेरो व्यवसायको अस्तित्वको लागि पर्याप्त ग्राहकहरू प्राप्त गर्न कठिनाइ हुनेछ</t>
@@ -1765,7 +1747,7 @@
     <t xml:space="preserve">p_hlth_hhs_measures__1</t>
   </si>
   <si>
-    <t xml:space="preserve">Trained our employees on Health, hygiene and sanitation</t>
+    <t xml:space="preserve">Trained employees on Health, hygiene and sanitation</t>
   </si>
   <si>
     <t xml:space="preserve">हाम्रा कर्मचारीहरुलाई स्वास्थ्य, सरसफाइ र स्वच्छतामा तालिम दिइयो </t>
@@ -1774,7 +1756,7 @@
     <t xml:space="preserve">p_hlth_hhs_measures__2</t>
   </si>
   <si>
-    <t xml:space="preserve">Maintained social distancing at our business premises</t>
+    <t xml:space="preserve">Maintained social distancing at business premises</t>
   </si>
   <si>
     <t xml:space="preserve">हाम्रो व्यवसाय परिसरमा सामाजिक दुरी बनाइयो</t>
@@ -1795,7 +1777,7 @@
     <t xml:space="preserve">p_hlth_hhs_measures__9</t>
   </si>
   <si>
-    <t xml:space="preserve">We didn't employ any health and sanitation related measures</t>
+    <t xml:space="preserve">Didn't employ any health and sanitation related measures</t>
   </si>
   <si>
     <t xml:space="preserve">हामीले स्वास्थ्य र सरसफाई सम्बन्धी कुनै उपायहरू प्रयोग गरेनौं</t>
@@ -3311,7 +3293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3340,12 +3322,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3425,15 +3401,19 @@
   </sheetPr>
   <dimension ref="A1:K393"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C169" activeCellId="0" sqref="C169"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J76" activeCellId="0" sqref="J76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>